<commit_message>
Fixed some typos in the compass driver Updated Excel sheet with driver status
</commit_message>
<xml_diff>
--- a/status_drivers.xlsx
+++ b/status_drivers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="13020"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="93">
   <si>
     <t>benedettelli-nxt2wifi.h</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>Unusable for EV3</t>
+  </si>
+  <si>
+    <t>SMUX</t>
+  </si>
+  <si>
+    <t>Supported</t>
   </si>
 </sst>
 </file>
@@ -351,96 +357,16 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="29">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1007,26 +933,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -1040,16 +966,19 @@
         <v>79</v>
       </c>
       <c r="E2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1063,16 +992,19 @@
         <v>84</v>
       </c>
       <c r="E3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" t="s">
         <v>87</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>80</v>
       </c>
-      <c r="I3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1085,14 +1017,17 @@
       <c r="D4" t="s">
         <v>83</v>
       </c>
-      <c r="G4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1105,11 +1040,14 @@
       <c r="D5" t="s">
         <v>83</v>
       </c>
-      <c r="G5" t="s">
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1122,13 +1060,16 @@
       <c r="D6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
         <v>83</v>
@@ -1137,15 +1078,18 @@
         <v>84</v>
       </c>
       <c r="E7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
         <v>83</v>
@@ -1153,8 +1097,11 @@
       <c r="D8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1167,8 +1114,11 @@
       <c r="D9" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1181,8 +1131,11 @@
       <c r="D10" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1195,8 +1148,11 @@
       <c r="D11" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1209,8 +1165,11 @@
       <c r="D12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1223,8 +1182,11 @@
       <c r="D13" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1237,8 +1199,11 @@
       <c r="D14" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1251,8 +1216,11 @@
       <c r="D15" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1265,8 +1233,11 @@
       <c r="D16" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1279,8 +1250,11 @@
       <c r="D17" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1294,10 +1268,13 @@
         <v>84</v>
       </c>
       <c r="E18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1310,8 +1287,11 @@
       <c r="D19" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1324,8 +1304,11 @@
       <c r="D20" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1338,8 +1321,11 @@
       <c r="D21" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1352,13 +1338,16 @@
       <c r="D22" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
         <v>83</v>
@@ -1366,13 +1355,16 @@
       <c r="D23" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
         <v>83</v>
@@ -1380,8 +1372,11 @@
       <c r="D24" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1394,8 +1389,11 @@
       <c r="D25" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1408,13 +1406,16 @@
       <c r="D26" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
         <v>83</v>
@@ -1422,8 +1423,11 @@
       <c r="D27" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1436,8 +1440,11 @@
       <c r="D28" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1450,8 +1457,11 @@
       <c r="D29" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1464,13 +1474,16 @@
       <c r="D30" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C31" t="s">
         <v>83</v>
@@ -1478,8 +1491,14 @@
       <c r="D31" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1492,8 +1511,11 @@
       <c r="D32" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -1506,8 +1528,11 @@
       <c r="D33" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1520,8 +1545,11 @@
       <c r="D34" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -1534,8 +1562,11 @@
       <c r="D35" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1548,8 +1579,11 @@
       <c r="D36" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -1562,8 +1596,11 @@
       <c r="D37" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -1576,8 +1613,11 @@
       <c r="D38" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -1590,8 +1630,11 @@
       <c r="D39" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -1604,8 +1647,11 @@
       <c r="D40" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -1618,8 +1664,11 @@
       <c r="D41" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -1632,8 +1681,11 @@
       <c r="D42" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -1646,8 +1698,11 @@
       <c r="D43" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -1660,8 +1715,11 @@
       <c r="D44" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -1674,8 +1732,11 @@
       <c r="D45" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -1688,8 +1749,11 @@
       <c r="D46" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -1702,8 +1766,11 @@
       <c r="D47" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -1716,8 +1783,11 @@
       <c r="D48" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -1730,8 +1800,11 @@
       <c r="D49" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -1744,8 +1817,11 @@
       <c r="D50" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -1759,10 +1835,13 @@
         <v>83</v>
       </c>
       <c r="E51" t="s">
+        <v>84</v>
+      </c>
+      <c r="F51" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -1776,10 +1855,13 @@
         <v>83</v>
       </c>
       <c r="E52" t="s">
+        <v>84</v>
+      </c>
+      <c r="F52" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -1793,10 +1875,13 @@
         <v>83</v>
       </c>
       <c r="E53" t="s">
+        <v>84</v>
+      </c>
+      <c r="F53" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -1809,8 +1894,11 @@
       <c r="D54" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -1824,10 +1912,13 @@
         <v>83</v>
       </c>
       <c r="E55" t="s">
+        <v>84</v>
+      </c>
+      <c r="F55" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -1840,8 +1931,11 @@
       <c r="D56" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -1854,8 +1948,11 @@
       <c r="D57" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -1868,8 +1965,11 @@
       <c r="D58" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -1882,8 +1982,11 @@
       <c r="D59" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -1896,8 +1999,11 @@
       <c r="D60" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -1910,8 +2016,11 @@
       <c r="D61" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -1924,8 +2033,11 @@
       <c r="D62" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -1938,8 +2050,11 @@
       <c r="D63" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -1952,8 +2067,11 @@
       <c r="D64" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -1966,8 +2084,11 @@
       <c r="D65" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -1980,8 +2101,11 @@
       <c r="D66" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -1994,8 +2118,11 @@
       <c r="D67" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -2008,8 +2135,11 @@
       <c r="D68" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>66</v>
       </c>
@@ -2022,8 +2152,11 @@
       <c r="D69" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -2036,8 +2169,11 @@
       <c r="D70" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -2050,8 +2186,11 @@
       <c r="D71" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -2064,8 +2203,11 @@
       <c r="D72" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -2078,8 +2220,11 @@
       <c r="D73" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -2093,10 +2238,13 @@
         <v>84</v>
       </c>
       <c r="E74" t="s">
+        <v>84</v>
+      </c>
+      <c r="F74" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -2109,8 +2257,11 @@
       <c r="D75" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E75" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -2123,8 +2274,11 @@
       <c r="D76" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -2138,10 +2292,13 @@
         <v>84</v>
       </c>
       <c r="E77" t="s">
+        <v>84</v>
+      </c>
+      <c r="F77" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>75</v>
       </c>
@@ -2155,6 +2312,9 @@
         <v>83</v>
       </c>
       <c r="E78" t="s">
+        <v>84</v>
+      </c>
+      <c r="F78" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2163,42 +2323,42 @@
   <mergeCells count="1">
     <mergeCell ref="C1:D1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:D78 E3 E53 E51 E77">
-    <cfRule type="cellIs" dxfId="36" priority="16" operator="equal">
+  <conditionalFormatting sqref="F53 F51 F77 E3:F3 C3:E78 F31">
+    <cfRule type="cellIs" dxfId="28" priority="16" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B78">
-    <cfRule type="cellIs" dxfId="34" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
       <formula>"No change"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="14" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
+  <conditionalFormatting sqref="F7">
+    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
+  <conditionalFormatting sqref="F18">
+    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E55">
+  <conditionalFormatting sqref="F55">
     <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2206,39 +2366,39 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+  <conditionalFormatting sqref="F52">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E78">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+  <conditionalFormatting sqref="F78">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="F74">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79:B81">
-      <formula1>G80:G82</formula1>
+      <formula1>H80:H82</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D78 C3:C81">
-      <formula1>$I$3:$I$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C81 D3:E78">
+      <formula1>$J$3:$J$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B78">
-      <formula1>$G$3:$G$5</formula1>
+      <formula1>$H$3:$H$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated driver status, with HTCS2 now completed. Added additional data (percentage complete, etc)
</commit_message>
<xml_diff>
--- a/status_drivers.xlsx
+++ b/status_drivers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="13020"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="95">
   <si>
     <t>benedettelli-nxt2wifi.h</t>
   </si>
@@ -306,13 +306,19 @@
   </si>
   <si>
     <t>Supported</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Todo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,6 +330,14 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -355,138 +369,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -634,6 +531,66 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -935,15 +892,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1100,6 +1057,13 @@
       <c r="E8" t="s">
         <v>84</v>
       </c>
+      <c r="H8" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8">
+        <f>COUNTA(B3:B78)</f>
+        <v>76</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1117,6 +1081,13 @@
       <c r="E9" t="s">
         <v>84</v>
       </c>
+      <c r="H9" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9">
+        <f>COUNTIF(B3:B78, "TBD")</f>
+        <v>57</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1134,6 +1105,17 @@
       <c r="E10" t="s">
         <v>84</v>
       </c>
+      <c r="H10" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="4">
+        <f>I8-I9</f>
+        <v>19</v>
+      </c>
+      <c r="J10" s="3">
+        <f>I10/I8</f>
+        <v>0.25</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1398,7 +1380,7 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
         <v>83</v>
@@ -2323,70 +2305,70 @@
   <mergeCells count="1">
     <mergeCell ref="C1:D1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F53 F51 F77 E3:F3 C3:E78 F31">
-    <cfRule type="cellIs" dxfId="28" priority="16" operator="equal">
+  <conditionalFormatting sqref="F53 F51 F77 E3:F3 C3:E78 F31 H8:H10">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B78">
-    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"No change"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F55">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52">
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F78">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F74">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>